<commit_message>
Fix all final bugs
</commit_message>
<xml_diff>
--- a/Estimation.xlsx
+++ b/Estimation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Estimation</t>
   </si>
@@ -38,17 +38,122 @@
     <t>Login page</t>
   </si>
   <si>
-    <t>2.1 login.html</t>
-  </si>
-  <si>
     <t>Build a structure of project (use Gulp, AngularJS, TypeScript)</t>
+  </si>
+  <si>
+    <t>User page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.1 UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.2 Reponsive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.1 UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.2 Reponsive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      3.3.1 Form add user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      3.3.2 Validate form</t>
+  </si>
+  <si>
+    <t>Group page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.1 UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.2 Reponsive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.3 Add group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      4.3.1 Form add group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      4.3.2 Validate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.4 Remove group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.5 Edit group</t>
+  </si>
+  <si>
+    <t>Total (hours)</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>AngularJS 1</t>
+  </si>
+  <si>
+    <t>TypeScript</t>
+  </si>
+  <si>
+    <t>Gulp</t>
+  </si>
+  <si>
+    <t>Technical skills</t>
+  </si>
+  <si>
+    <t>PouchDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.4 Remember Me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.3 Login/Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.3 Search/Paging/Sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.4 Add user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.5 Remove user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.6 Edit user</t>
+  </si>
+  <si>
+    <t>Permission (Admin/Editor/View)</t>
+  </si>
+  <si>
+    <t>Configuration page (database, expire login time)</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
+    <t>SASS (custom + Bootstrap 3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,13 +161,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,8 +224,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,60 +550,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5">
+        <f xml:space="preserve"> SUM(C3:C27)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
+      <c r="E5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>5</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="4">
+        <v>3</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>6</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="4">
+        <v>3</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>